<commit_message>
Changed baseline cov to same
</commit_message>
<xml_diff>
--- a/applications/demo/data/regional/demoregion3_input.xlsx
+++ b/applications/demo/data/regional/demoregion3_input.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samhainsworth/Desktop/github_projects/Nutrition/applications/demo/data/regional/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{B8296569-6252-AB44-BC2E-EC2AE2B9F30A}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{88B66F9D-1191-7746-BADF-1F7F5074848D}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="961" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4145,8 +4145,8 @@
   </sheetPr>
   <dimension ref="A1:E62"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4411,7 +4411,7 @@
         <v>92</v>
       </c>
       <c r="C36" s="25">
-        <v>25</v>
+        <v>18.75</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -4419,7 +4419,7 @@
         <v>91</v>
       </c>
       <c r="C37" s="25">
-        <v>43</v>
+        <v>32.25</v>
       </c>
       <c r="D37" s="20"/>
       <c r="E37" s="21"/>
@@ -4429,7 +4429,7 @@
         <v>90</v>
       </c>
       <c r="C38" s="25">
-        <v>67</v>
+        <v>50.25</v>
       </c>
       <c r="D38" s="20"/>
       <c r="E38" s="20"/>
@@ -4439,7 +4439,7 @@
         <v>172</v>
       </c>
       <c r="C39" s="25">
-        <v>4.01</v>
+        <v>3.0074999999999998</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -9857,7 +9857,7 @@
   <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -9949,7 +9949,7 @@
         <v>63</v>
       </c>
       <c r="B6" s="71">
-        <v>0</v>
+        <v>0.36</v>
       </c>
       <c r="C6" s="71">
         <v>0.95</v>
@@ -10048,7 +10048,7 @@
         <v>57</v>
       </c>
       <c r="B13" s="71">
-        <v>0</v>
+        <v>0.34599999999999997</v>
       </c>
       <c r="C13" s="71">
         <v>0.95</v>
@@ -10063,7 +10063,7 @@
         <v>47</v>
       </c>
       <c r="B14" s="71">
-        <v>0</v>
+        <v>0.80800000000000005</v>
       </c>
       <c r="C14" s="71">
         <v>0.95</v>
@@ -10152,7 +10152,7 @@
         <v>34</v>
       </c>
       <c r="B20" s="71">
-        <v>0</v>
+        <v>0.50800000000000001</v>
       </c>
       <c r="C20" s="71">
         <v>0.95</v>
@@ -10197,7 +10197,7 @@
         <v>138</v>
       </c>
       <c r="B23" s="71">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="C23" s="71">
         <v>0.95</v>
@@ -10212,7 +10212,7 @@
         <v>59</v>
       </c>
       <c r="B24" s="71">
-        <v>0</v>
+        <v>0.3538</v>
       </c>
       <c r="C24" s="71">
         <v>0.95</v>
@@ -10270,7 +10270,7 @@
         <v>28</v>
       </c>
       <c r="B28" s="71">
-        <v>0</v>
+        <v>0.89970000000000006</v>
       </c>
       <c r="C28" s="71">
         <v>0.95</v>
@@ -10284,7 +10284,7 @@
         <v>83</v>
       </c>
       <c r="B29" s="71">
-        <v>0</v>
+        <v>0.80700000000000005</v>
       </c>
       <c r="C29" s="71">
         <v>0.95</v>
@@ -10298,7 +10298,7 @@
         <v>82</v>
       </c>
       <c r="B30" s="71">
-        <v>0</v>
+        <v>0.73199999999999998</v>
       </c>
       <c r="C30" s="71">
         <v>0.95</v>
@@ -10312,7 +10312,7 @@
         <v>81</v>
       </c>
       <c r="B31" s="71">
-        <v>0</v>
+        <v>0.316</v>
       </c>
       <c r="C31" s="71">
         <v>0.95</v>
@@ -10326,7 +10326,7 @@
         <v>79</v>
       </c>
       <c r="B32" s="71">
-        <v>0</v>
+        <v>0.59699999999999998</v>
       </c>
       <c r="C32" s="71">
         <v>0.95</v>
@@ -10340,7 +10340,7 @@
         <v>80</v>
       </c>
       <c r="B33" s="71">
-        <v>0</v>
+        <v>0.19900000000000001</v>
       </c>
       <c r="C33" s="71">
         <v>0.95</v>
@@ -10355,7 +10355,7 @@
         <v>85</v>
       </c>
       <c r="B34" s="71">
-        <v>0</v>
+        <v>0.13400000000000001</v>
       </c>
       <c r="C34" s="71">
         <v>0.95</v>

</xml_diff>

<commit_message>
changed baseling cov to 0, made parallel run
</commit_message>
<xml_diff>
--- a/applications/demo/data/regional/demoregion3_input.xlsx
+++ b/applications/demo/data/regional/demoregion3_input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samhainsworth/Desktop/github_projects/Nutrition/applications/demo/data/regional/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{88B66F9D-1191-7746-BADF-1F7F5074848D}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{599D12E2-B8E2-4541-8244-34A3CA0136C5}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="961" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="961" firstSheet="6" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year population inputs" sheetId="1" r:id="rId1"/>
@@ -4145,7 +4145,7 @@
   </sheetPr>
   <dimension ref="A1:E62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
@@ -9856,8 +9856,8 @@
   </sheetPr>
   <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -9949,7 +9949,7 @@
         <v>63</v>
       </c>
       <c r="B6" s="71">
-        <v>0.36</v>
+        <v>0</v>
       </c>
       <c r="C6" s="71">
         <v>0.95</v>
@@ -10048,7 +10048,7 @@
         <v>57</v>
       </c>
       <c r="B13" s="71">
-        <v>0.34599999999999997</v>
+        <v>0</v>
       </c>
       <c r="C13" s="71">
         <v>0.95</v>
@@ -10063,7 +10063,7 @@
         <v>47</v>
       </c>
       <c r="B14" s="71">
-        <v>0.80800000000000005</v>
+        <v>0</v>
       </c>
       <c r="C14" s="71">
         <v>0.95</v>
@@ -10152,7 +10152,7 @@
         <v>34</v>
       </c>
       <c r="B20" s="71">
-        <v>0.50800000000000001</v>
+        <v>0</v>
       </c>
       <c r="C20" s="71">
         <v>0.95</v>
@@ -10197,7 +10197,7 @@
         <v>138</v>
       </c>
       <c r="B23" s="71">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="C23" s="71">
         <v>0.95</v>
@@ -10212,7 +10212,7 @@
         <v>59</v>
       </c>
       <c r="B24" s="71">
-        <v>0.3538</v>
+        <v>0</v>
       </c>
       <c r="C24" s="71">
         <v>0.95</v>
@@ -10270,7 +10270,7 @@
         <v>28</v>
       </c>
       <c r="B28" s="71">
-        <v>0.89970000000000006</v>
+        <v>0</v>
       </c>
       <c r="C28" s="71">
         <v>0.95</v>
@@ -10284,7 +10284,7 @@
         <v>83</v>
       </c>
       <c r="B29" s="71">
-        <v>0.80700000000000005</v>
+        <v>0</v>
       </c>
       <c r="C29" s="71">
         <v>0.95</v>
@@ -10298,7 +10298,7 @@
         <v>82</v>
       </c>
       <c r="B30" s="71">
-        <v>0.73199999999999998</v>
+        <v>0</v>
       </c>
       <c r="C30" s="71">
         <v>0.95</v>
@@ -10312,7 +10312,7 @@
         <v>81</v>
       </c>
       <c r="B31" s="71">
-        <v>0.316</v>
+        <v>0</v>
       </c>
       <c r="C31" s="71">
         <v>0.95</v>
@@ -10326,7 +10326,7 @@
         <v>79</v>
       </c>
       <c r="B32" s="71">
-        <v>0.59699999999999998</v>
+        <v>0</v>
       </c>
       <c r="C32" s="71">
         <v>0.95</v>
@@ -10340,7 +10340,7 @@
         <v>80</v>
       </c>
       <c r="B33" s="71">
-        <v>0.19900000000000001</v>
+        <v>0</v>
       </c>
       <c r="C33" s="71">
         <v>0.95</v>
@@ -10355,7 +10355,7 @@
         <v>85</v>
       </c>
       <c r="B34" s="71">
-        <v>0.13400000000000001</v>
+        <v>0</v>
       </c>
       <c r="C34" s="71">
         <v>0.95</v>

</xml_diff>

<commit_message>
Changed to nonzero cov
</commit_message>
<xml_diff>
--- a/applications/demo/data/regional/demoregion3_input.xlsx
+++ b/applications/demo/data/regional/demoregion3_input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samhainsworth/Desktop/github_projects/Nutrition/applications/demo/data/regional/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{599D12E2-B8E2-4541-8244-34A3CA0136C5}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{5D40171C-7B40-3B46-ABE7-502594F2DC32}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="961" firstSheet="6" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="961" firstSheet="6" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year population inputs" sheetId="1" r:id="rId1"/>
@@ -9857,7 +9857,7 @@
   <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -9949,7 +9949,7 @@
         <v>63</v>
       </c>
       <c r="B6" s="71">
-        <v>0</v>
+        <v>0.36</v>
       </c>
       <c r="C6" s="71">
         <v>0.95</v>
@@ -10048,7 +10048,7 @@
         <v>57</v>
       </c>
       <c r="B13" s="71">
-        <v>0</v>
+        <v>0.34599999999999997</v>
       </c>
       <c r="C13" s="71">
         <v>0.95</v>
@@ -10063,7 +10063,7 @@
         <v>47</v>
       </c>
       <c r="B14" s="71">
-        <v>0</v>
+        <v>0.80800000000000005</v>
       </c>
       <c r="C14" s="71">
         <v>0.95</v>
@@ -10152,7 +10152,7 @@
         <v>34</v>
       </c>
       <c r="B20" s="71">
-        <v>0</v>
+        <v>0.50800000000000001</v>
       </c>
       <c r="C20" s="71">
         <v>0.95</v>
@@ -10197,7 +10197,7 @@
         <v>138</v>
       </c>
       <c r="B23" s="71">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="C23" s="71">
         <v>0.95</v>
@@ -10212,7 +10212,7 @@
         <v>59</v>
       </c>
       <c r="B24" s="71">
-        <v>0</v>
+        <v>0.3538</v>
       </c>
       <c r="C24" s="71">
         <v>0.95</v>
@@ -10270,7 +10270,7 @@
         <v>28</v>
       </c>
       <c r="B28" s="71">
-        <v>0</v>
+        <v>0.89970000000000006</v>
       </c>
       <c r="C28" s="71">
         <v>0.95</v>
@@ -10284,7 +10284,7 @@
         <v>83</v>
       </c>
       <c r="B29" s="71">
-        <v>0</v>
+        <v>0.80700000000000005</v>
       </c>
       <c r="C29" s="71">
         <v>0.95</v>
@@ -10298,7 +10298,7 @@
         <v>82</v>
       </c>
       <c r="B30" s="71">
-        <v>0</v>
+        <v>0.73199999999999998</v>
       </c>
       <c r="C30" s="71">
         <v>0.95</v>
@@ -10312,7 +10312,7 @@
         <v>81</v>
       </c>
       <c r="B31" s="71">
-        <v>0</v>
+        <v>0.316</v>
       </c>
       <c r="C31" s="71">
         <v>0.95</v>
@@ -10326,7 +10326,7 @@
         <v>79</v>
       </c>
       <c r="B32" s="71">
-        <v>0</v>
+        <v>0.59699999999999998</v>
       </c>
       <c r="C32" s="71">
         <v>0.95</v>
@@ -10340,7 +10340,7 @@
         <v>80</v>
       </c>
       <c r="B33" s="71">
-        <v>0</v>
+        <v>0.19900000000000001</v>
       </c>
       <c r="C33" s="71">
         <v>0.95</v>
@@ -10355,7 +10355,7 @@
         <v>85</v>
       </c>
       <c r="B34" s="71">
-        <v>0</v>
+        <v>0.13400000000000001</v>
       </c>
       <c r="C34" s="71">
         <v>0.95</v>

</xml_diff>

<commit_message>
Changed 3rd test region to have 0 baseline spending, updated test
</commit_message>
<xml_diff>
--- a/applications/demo/data/regional/demoregion3_input.xlsx
+++ b/applications/demo/data/regional/demoregion3_input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samhainsworth/Desktop/github_projects/Nutrition/applications/demo/data/regional/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{5D40171C-7B40-3B46-ABE7-502594F2DC32}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{51B16486-16FD-C944-84FB-76644F8D1CE7}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="961" firstSheet="6" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="961" firstSheet="6" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year population inputs" sheetId="1" r:id="rId1"/>
@@ -9856,8 +9856,8 @@
   </sheetPr>
   <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -9949,7 +9949,7 @@
         <v>63</v>
       </c>
       <c r="B6" s="71">
-        <v>0.36</v>
+        <v>0</v>
       </c>
       <c r="C6" s="71">
         <v>0.95</v>
@@ -10048,7 +10048,7 @@
         <v>57</v>
       </c>
       <c r="B13" s="71">
-        <v>0.34599999999999997</v>
+        <v>0</v>
       </c>
       <c r="C13" s="71">
         <v>0.95</v>
@@ -10063,7 +10063,7 @@
         <v>47</v>
       </c>
       <c r="B14" s="71">
-        <v>0.80800000000000005</v>
+        <v>0</v>
       </c>
       <c r="C14" s="71">
         <v>0.95</v>
@@ -10152,7 +10152,7 @@
         <v>34</v>
       </c>
       <c r="B20" s="71">
-        <v>0.50800000000000001</v>
+        <v>0</v>
       </c>
       <c r="C20" s="71">
         <v>0.95</v>
@@ -10197,7 +10197,7 @@
         <v>138</v>
       </c>
       <c r="B23" s="71">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="C23" s="71">
         <v>0.95</v>
@@ -10212,7 +10212,7 @@
         <v>59</v>
       </c>
       <c r="B24" s="71">
-        <v>0.3538</v>
+        <v>0</v>
       </c>
       <c r="C24" s="71">
         <v>0.95</v>
@@ -10270,7 +10270,7 @@
         <v>28</v>
       </c>
       <c r="B28" s="71">
-        <v>0.89970000000000006</v>
+        <v>0</v>
       </c>
       <c r="C28" s="71">
         <v>0.95</v>
@@ -10284,7 +10284,7 @@
         <v>83</v>
       </c>
       <c r="B29" s="71">
-        <v>0.80700000000000005</v>
+        <v>0</v>
       </c>
       <c r="C29" s="71">
         <v>0.95</v>
@@ -10298,7 +10298,7 @@
         <v>82</v>
       </c>
       <c r="B30" s="71">
-        <v>0.73199999999999998</v>
+        <v>0</v>
       </c>
       <c r="C30" s="71">
         <v>0.95</v>
@@ -10312,7 +10312,7 @@
         <v>81</v>
       </c>
       <c r="B31" s="71">
-        <v>0.316</v>
+        <v>0</v>
       </c>
       <c r="C31" s="71">
         <v>0.95</v>
@@ -10326,7 +10326,7 @@
         <v>79</v>
       </c>
       <c r="B32" s="71">
-        <v>0.59699999999999998</v>
+        <v>0</v>
       </c>
       <c r="C32" s="71">
         <v>0.95</v>
@@ -10340,7 +10340,7 @@
         <v>80</v>
       </c>
       <c r="B33" s="71">
-        <v>0.19900000000000001</v>
+        <v>0</v>
       </c>
       <c r="C33" s="71">
         <v>0.95</v>
@@ -10355,7 +10355,7 @@
         <v>85</v>
       </c>
       <c r="B34" s="71">
-        <v>0.13400000000000001</v>
+        <v>0</v>
       </c>
       <c r="C34" s="71">
         <v>0.95</v>

</xml_diff>